<commit_message>
The framework is perfectly setup for script development. Started working on a smoke script for Amazon
</commit_message>
<xml_diff>
--- a/framework-design/Resources/DriverFile/Driver File.xlsx
+++ b/framework-design/Resources/DriverFile/Driver File.xlsx
@@ -67,9 +67,6 @@
     <t>\\Resources\\ModuleFiles\\ElavonScripts.xlsx</t>
   </si>
   <si>
-    <t>\\Resources\\ModuleFiles\\Job Search.xlsx</t>
-  </si>
-  <si>
     <t>\\Resources\\ObjectRepository\\objects.properties</t>
   </si>
   <si>
@@ -77,16 +74,27 @@
   </si>
   <si>
     <t>\\Resources\\ObjectRepository\\ElavonObjects.properties</t>
+  </si>
+  <si>
+    <t>\\Resources\\ModuleFiles\\JobSearch.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,16 +117,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,7 +432,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +479,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -488,7 +499,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -504,11 +515,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Made several changes to the repository. 1. Introduced block files- Block files consist of self-contained blocks of keywords that can be reused 2. Developed keyword for improved wait times using fluent wait 3. Removed unnecessary files. 4. Included sample reports
</commit_message>
<xml_diff>
--- a/framework-design/Resources/DriverFile/Driver File.xlsx
+++ b/framework-design/Resources/DriverFile/Driver File.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
-  <si>
-    <t>Sample Script</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Module Name</t>
   </si>
@@ -37,30 +34,9 @@
     <t>Module File Name</t>
   </si>
   <si>
-    <t>sampleModuleFile</t>
-  </si>
-  <si>
     <t>Site Name</t>
   </si>
   <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>ElavonScripts</t>
-  </si>
-  <si>
-    <t>newsLive</t>
-  </si>
-  <si>
-    <t>Job Search</t>
-  </si>
-  <si>
-    <t>jobSearch</t>
-  </si>
-  <si>
     <t>AmazonSmokeTest</t>
   </si>
   <si>
@@ -70,31 +46,13 @@
     <t>BlockFile</t>
   </si>
   <si>
-    <t>AmazonBlocks</t>
-  </si>
-  <si>
-    <t>objects.properties</t>
-  </si>
-  <si>
-    <t>ElavonObjects.properties</t>
-  </si>
-  <si>
-    <t>JobSearchObjects.properties</t>
-  </si>
-  <si>
     <t>AmazonObjects.properties</t>
   </si>
   <si>
     <t>AmazonSmokeTest.xlsx</t>
   </si>
   <si>
-    <t>JobSearch.xlsx</t>
-  </si>
-  <si>
-    <t>ElavonScripts.xlsx</t>
-  </si>
-  <si>
-    <t>sampleModuleFile.xlsx</t>
+    <t>AmazonBlocks.xlsx</t>
   </si>
 </sst>
 </file>
@@ -436,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,108 +413,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>